<commit_message>
Updated Activities column in the gantt chart, and student id section of the software design document
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Courses\2810ICT\2024\2810-7810-workspace\Group_Project\M1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9675C1-8042-4DA2-BC81-E829931B8A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF150565-4C38-4C23-B142-797DB78985F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -40,84 +40,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>PERIODS</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -207,34 +129,10 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
     <t>Activity 34</t>
   </si>
   <si>
     <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
   </si>
   <si>
     <t>Plan
@@ -262,6 +160,108 @@
   </si>
   <si>
     <t>Activity No. and Name</t>
+  </si>
+  <si>
+    <t>Nutrient Analyzer</t>
+  </si>
+  <si>
+    <t>1. Project Objectives Documentation</t>
+  </si>
+  <si>
+    <t>2. Project Scope Definition</t>
+  </si>
+  <si>
+    <t>3. Stakeholder Identification</t>
+  </si>
+  <si>
+    <t>4.Design</t>
+  </si>
+  <si>
+    <t>4.1 Design Documentation</t>
+  </si>
+  <si>
+    <t>4.2 User Interface (UI) Design</t>
+  </si>
+  <si>
+    <t>4.3 User Experience (UX) Design</t>
+  </si>
+  <si>
+    <t>5. Data Preprocessing</t>
+  </si>
+  <si>
+    <t>5.1Nutritional_Food_Database.csv Import</t>
+  </si>
+  <si>
+    <t>5.2 Data Cleaning and Validation</t>
+  </si>
+  <si>
+    <t>5.3 Data Integration</t>
+  </si>
+  <si>
+    <t>6. Development</t>
+  </si>
+  <si>
+    <t>6.1 Desktop Application Development</t>
+  </si>
+  <si>
+    <t>6.2 Feature Implementation</t>
+  </si>
+  <si>
+    <t>6.2.1 Food Search</t>
+  </si>
+  <si>
+    <t>6.2.2 Nutrition Breakdown</t>
+  </si>
+  <si>
+    <t>6.2.3 Nutrition Range Filter</t>
+  </si>
+  <si>
+    <t>6.2.4 Nutrition Level Filter</t>
+  </si>
+  <si>
+    <t>6.2.5 Additional Feature</t>
+  </si>
+  <si>
+    <t>6.2.6 Graphical User Interface (GUI) Development</t>
+  </si>
+  <si>
+    <t>7 Testing and Validation</t>
+  </si>
+  <si>
+    <t>7.1 Unit Testing</t>
+  </si>
+  <si>
+    <t>7.2 Integration Testing</t>
+  </si>
+  <si>
+    <t>7.3 User Acceptance Testing (UAT)</t>
+  </si>
+  <si>
+    <t>7.4 Usability Testing</t>
+  </si>
+  <si>
+    <t>8. Documentation</t>
+  </si>
+  <si>
+    <t>8.2 Design Documentation</t>
+  </si>
+  <si>
+    <t>8.1 Project Plan Documentation</t>
+  </si>
+  <si>
+    <t>8.3 User Manual</t>
+  </si>
+  <si>
+    <t>9. Project Closure</t>
+  </si>
+  <si>
+    <t>9.1 Final Report</t>
+  </si>
+  <si>
+    <t>9.2 Lessons Learned</t>
+  </si>
+  <si>
+    <t>9.3 Project Evaluation</t>
   </si>
 </sst>
 </file>
@@ -846,6 +846,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1079,26 +1083,26 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.796875" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="5" max="5" width="5.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.296875" style="4" customWidth="1"/>
+    <col min="8" max="27" width="2.796875" style="1"/>
+    <col min="42" max="42" width="2.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:67" ht="59.95" customHeight="1" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1106,21 +1110,21 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:67" ht="33.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="21" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="30" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1128,21 +1132,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="14"/>
       <c r="Q2" s="30" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="15"/>
       <c r="V2" s="34" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="W2" s="35"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="36"/>
       <c r="Z2" s="16"/>
       <c r="AA2" s="34" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="AB2" s="35"/>
       <c r="AC2" s="35"/>
@@ -1152,7 +1156,7 @@
       <c r="AG2" s="36"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="20"/>
       <c r="AK2" s="20"/>
@@ -1162,24 +1166,24 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>0</v>
@@ -1204,7 +1208,7 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:67" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1392,19 +1396,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
       <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5">
         <v>0</v>
       </c>
@@ -1412,12 +1414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
@@ -1428,9 +1430,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="23" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1440,9 +1442,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="23" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1452,9 +1454,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1464,9 +1466,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1476,9 +1478,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1488,9 +1490,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1500,9 +1502,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1512,9 +1514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1524,9 +1526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
@@ -1536,9 +1538,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1548,9 +1550,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1560,9 +1562,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1572,9 +1574,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1584,9 +1586,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1596,9 +1598,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1608,9 +1610,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1620,9 +1622,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="23" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1632,9 +1634,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1644,9 +1646,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="23" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1656,9 +1658,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1668,9 +1670,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1680,9 +1682,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="23" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1692,9 +1694,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1704,9 +1706,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="23" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1716,9 +1718,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1728,9 +1730,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="23" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1740,9 +1742,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="23" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1752,9 +1754,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="23" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1764,9 +1766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="23" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1776,9 +1778,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="23" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1788,9 +1790,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="23" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1800,9 +1802,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="23" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1812,9 +1814,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="23" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1905,6 +1907,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{adaa4be3-f650-4692-881a-64ae220cbceb}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+  <clbl:label id="{adaa4be3-f650-4692-881a-64ae220cbceb}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update the System Vision, User Requirements and Software Requirements
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Courses\2810ICT\2024\2810-7810-workspace\Group_Project\M1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/simarjotkaur_griffithuni_edu_au/Documents/Desktop/Trim 2 Assignments/2810ICT SoftTech/Milestone1_Group62/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9675C1-8042-4DA2-BC81-E829931B8A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{1B9675C1-8042-4DA2-BC81-E829931B8A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F782EB37-7C63-4C57-96AE-63EC88FD3B5E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -40,84 +40,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>PERIODS</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -207,34 +129,10 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
     <t>Activity 34</t>
   </si>
   <si>
     <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
   </si>
   <si>
     <t>Plan
@@ -262,6 +160,108 @@
   </si>
   <si>
     <t>Activity No. and Name</t>
+  </si>
+  <si>
+    <t>Nutrient Analyzer</t>
+  </si>
+  <si>
+    <t>1. Project Objectives Documentation</t>
+  </si>
+  <si>
+    <t>2. Project Scope Definition</t>
+  </si>
+  <si>
+    <t>3. Stakeholder Identification</t>
+  </si>
+  <si>
+    <t>4.Design</t>
+  </si>
+  <si>
+    <t>4.1 Design Documentation</t>
+  </si>
+  <si>
+    <t>4.2 User Interface (UI) Design</t>
+  </si>
+  <si>
+    <t>4.3 User Experience (UX) Design</t>
+  </si>
+  <si>
+    <t>5. Data Preprocessing</t>
+  </si>
+  <si>
+    <t>5.1Nutritional_Food_Database.csv Import</t>
+  </si>
+  <si>
+    <t>5.2 Data Cleaning and Validation</t>
+  </si>
+  <si>
+    <t>5.3 Data Integration</t>
+  </si>
+  <si>
+    <t>6. Development</t>
+  </si>
+  <si>
+    <t>6.1 Desktop Application Development</t>
+  </si>
+  <si>
+    <t>6.2 Feature Implementation</t>
+  </si>
+  <si>
+    <t>6.2.1 Food Search</t>
+  </si>
+  <si>
+    <t>6.2.2 Nutrition Breakdown</t>
+  </si>
+  <si>
+    <t>6.2.3 Nutrition Range Filter</t>
+  </si>
+  <si>
+    <t>6.2.4 Nutrition Level Filter</t>
+  </si>
+  <si>
+    <t>6.2.5 Additional Feature</t>
+  </si>
+  <si>
+    <t>6.2.6 Graphical User Interface (GUI) Development</t>
+  </si>
+  <si>
+    <t>7 Testing and Validation</t>
+  </si>
+  <si>
+    <t>7.1 Unit Testing</t>
+  </si>
+  <si>
+    <t>7.2 Integration Testing</t>
+  </si>
+  <si>
+    <t>7.3 User Acceptance Testing (UAT)</t>
+  </si>
+  <si>
+    <t>7.4 Usability Testing</t>
+  </si>
+  <si>
+    <t>8. Documentation</t>
+  </si>
+  <si>
+    <t>8.2 Design Documentation</t>
+  </si>
+  <si>
+    <t>8.1 Project Plan Documentation</t>
+  </si>
+  <si>
+    <t>8.3 User Manual</t>
+  </si>
+  <si>
+    <t>9. Project Closure</t>
+  </si>
+  <si>
+    <t>9.1 Final Report</t>
+  </si>
+  <si>
+    <t>9.2 Lessons Learned</t>
+  </si>
+  <si>
+    <t>9.3 Project Evaluation</t>
   </si>
 </sst>
 </file>
@@ -846,6 +846,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1079,26 +1083,26 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.796875" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="5" max="5" width="5.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.296875" style="4" customWidth="1"/>
+    <col min="8" max="27" width="2.796875" style="1"/>
+    <col min="42" max="42" width="2.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:67" ht="59.95" customHeight="1" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1106,21 +1110,21 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:67" ht="33.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="21" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="30" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1128,21 +1132,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="14"/>
       <c r="Q2" s="30" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="15"/>
       <c r="V2" s="34" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="W2" s="35"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="36"/>
       <c r="Z2" s="16"/>
       <c r="AA2" s="34" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="AB2" s="35"/>
       <c r="AC2" s="35"/>
@@ -1152,7 +1156,7 @@
       <c r="AG2" s="36"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="20"/>
       <c r="AK2" s="20"/>
@@ -1162,24 +1166,24 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>0</v>
@@ -1204,7 +1208,7 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:67" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1392,19 +1396,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
       <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5">
         <v>0</v>
       </c>
@@ -1412,12 +1414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
@@ -1428,9 +1430,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="23" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1440,9 +1442,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="23" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1452,9 +1454,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1464,9 +1466,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1476,9 +1478,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1488,9 +1490,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1500,9 +1502,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1512,9 +1514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1524,9 +1526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
@@ -1536,9 +1538,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:67" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1548,9 +1550,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1560,9 +1562,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1572,9 +1574,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1584,9 +1586,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1596,9 +1598,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1608,9 +1610,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1620,9 +1622,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="23" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1632,9 +1634,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1644,9 +1646,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="23" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1656,9 +1658,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1668,9 +1670,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1680,9 +1682,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="23" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1692,9 +1694,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1704,9 +1706,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="23" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1716,9 +1718,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1728,9 +1730,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="23" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1740,9 +1742,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="23" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1752,9 +1754,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="23" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1764,9 +1766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="23" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1776,9 +1778,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="23" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1788,9 +1790,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="23" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1800,9 +1802,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="23" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1812,9 +1814,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="23" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>

</xml_diff>

<commit_message>
updated image of Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh Patel\Desktop\Milestone upload files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh Patel\Desktop\Tri2\Software_Technologies\Milestone2_Group62\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A816B22-A3AE-4644-9F15-DB017DBE27F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F90885E-6DE9-45F2-A2EB-0BE1EFBA3CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PERIODS</t>
   </si>
@@ -132,22 +132,6 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>Plan
-Start</t>
-  </si>
-  <si>
-    <t>Actual
-Duration</t>
-  </si>
-  <si>
-    <t>Actual
-Start</t>
-  </si>
-  <si>
-    <t>Plan
-Duration</t>
-  </si>
-  <si>
     <t>Percent
 Complete</t>
   </si>
@@ -204,18 +188,6 @@
     <t>5.1 Perform Unit Testing</t>
   </si>
   <si>
-    <t>5.2 Perform Integration Testing</t>
-  </si>
-  <si>
-    <t>5.3 Perform Usability Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.4 Perform System Testing</t>
-  </si>
-  <si>
-    <t>5.5 Performing final system</t>
-  </si>
-  <si>
     <t>6. Documentation and Final Reporting</t>
   </si>
   <si>
@@ -229,13 +201,59 @@
   </si>
   <si>
     <t>Nutrient Analyzer</t>
+  </si>
+  <si>
+    <t>Plan (in days)
+Start</t>
+  </si>
+  <si>
+    <t>Plan(in days)
+Duration</t>
+  </si>
+  <si>
+    <t>Actual(in days)
+Start</t>
+  </si>
+  <si>
+    <t>Actual
+Duration(in days)</t>
+  </si>
+  <si>
+    <r>
+      <t>5.2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Perform Statement Coverage Testing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Perform Branch Coverage Testing</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -351,6 +369,19 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -539,7 +570,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,12 +643,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -639,17 +682,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1164,10 +1198,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO42"/>
+  <dimension ref="B1:BO40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BT17" sqref="BT17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1185,7 +1219,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1194,49 +1228,49 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>4</v>
@@ -1250,23 +1284,23 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>0</v>
@@ -1292,12 +1326,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1481,7 +1515,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1501,7 +1535,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1521,7 +1555,7 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -1541,7 +1575,7 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -1561,7 +1595,7 @@
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5">
         <v>4</v>
@@ -1581,7 +1615,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5">
         <v>4</v>
@@ -1601,7 +1635,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5">
         <v>5</v>
@@ -1621,7 +1655,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>7</v>
@@ -1641,7 +1675,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <v>7</v>
@@ -1661,7 +1695,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5">
         <v>9</v>
@@ -1681,7 +1715,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6">
         <v>11</v>
@@ -1701,7 +1735,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5">
         <v>11</v>
@@ -1721,7 +1755,7 @@
     </row>
     <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C17" s="5">
         <v>13</v>
@@ -1741,7 +1775,7 @@
     </row>
     <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5">
         <v>17</v>
@@ -1761,19 +1795,19 @@
     </row>
     <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5">
         <v>20</v>
       </c>
-      <c r="D19" s="5">
-        <v>10</v>
+      <c r="D19" s="37">
+        <v>6</v>
       </c>
       <c r="E19" s="5">
         <v>20</v>
       </c>
-      <c r="F19" s="5">
-        <v>10</v>
+      <c r="F19" s="37">
+        <v>6</v>
       </c>
       <c r="G19" s="22">
         <v>1</v>
@@ -1781,7 +1815,7 @@
     </row>
     <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5">
         <v>20</v>
@@ -1801,7 +1835,7 @@
     </row>
     <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5">
         <v>22</v>
@@ -1821,15 +1855,15 @@
     </row>
     <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="5">
+        <v>35</v>
+      </c>
+      <c r="C22" s="37">
         <v>24</v>
       </c>
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="37">
         <v>24</v>
       </c>
       <c r="F22" s="5">
@@ -1841,15 +1875,15 @@
     </row>
     <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="5">
+        <v>25</v>
+      </c>
+      <c r="C23" s="37">
         <v>26</v>
       </c>
       <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="37">
         <v>26</v>
       </c>
       <c r="F23" s="5">
@@ -1861,19 +1895,19 @@
     </row>
     <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="5">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="C24" s="37">
+        <v>26</v>
       </c>
       <c r="D24" s="5">
-        <v>2</v>
-      </c>
-      <c r="E24" s="5">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="E24" s="37">
+        <v>26</v>
       </c>
       <c r="F24" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="22">
         <v>1</v>
@@ -1881,19 +1915,19 @@
     </row>
     <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="5">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C25" s="37">
+        <v>27</v>
       </c>
       <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="E25" s="37">
+        <v>27</v>
       </c>
       <c r="F25" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="22">
         <v>1</v>
@@ -1901,55 +1935,71 @@
     </row>
     <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="5">
-        <v>30</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5">
-        <v>30</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="5">
-        <v>31</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5">
-        <v>31</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="22">
-        <v>1</v>
-      </c>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
     </row>
     <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="22">
-        <v>0</v>
-      </c>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
     </row>
     <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
@@ -2259,13 +2309,7 @@
       <c r="Z39"/>
       <c r="AA39"/>
     </row>
-    <row r="40" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
+    <row r="40" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -2287,69 +2331,19 @@
       <c r="Z40"/>
       <c r="AA40"/>
     </row>
-    <row r="41" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-    </row>
-    <row r="42" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-      <c r="X42"/>
-      <c r="Y42"/>
-      <c r="Z42"/>
-      <c r="AA42"/>
-    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="H4:BO4">
@@ -2357,7 +2351,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO16 H17:Q17 T17:BO17 H18:BO28">
+  <conditionalFormatting sqref="H5:BO16 H17:Q17 T17:BO17 H18:BO26">
     <cfRule type="expression" dxfId="15" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>